<commit_message>
Correcao no calculo da forma
</commit_message>
<xml_diff>
--- a/others/Forma.xlsx
+++ b/others/Forma.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Dia</t>
   </si>
@@ -218,13 +218,17 @@
   <si>
     <t>Carregar nas setas para gerar diferentes valores aleatórios para os mins actividade/dia.</t>
   </si>
+  <si>
+    <t>exp</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -691,20 +695,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -721,9 +719,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -768,30 +763,60 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -819,24 +844,6 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -855,16 +862,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -900,13 +907,13 @@
           <xdr:col>10</xdr:col>
           <xdr:colOff>304800</xdr:colOff>
           <xdr:row>21</xdr:row>
-          <xdr:rowOff>9524</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>12</xdr:col>
           <xdr:colOff>238125</xdr:colOff>
           <xdr:row>23</xdr:row>
-          <xdr:rowOff>190499</xdr:rowOff>
+          <xdr:rowOff>190500</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1226,8 +1233,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1238,708 +1245,779 @@
     <col min="5" max="5" width="12" style="1" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="15.28515625" style="1" customWidth="1"/>
-    <col min="8" max="16" width="9.140625" style="1"/>
+    <col min="8" max="8" width="9.140625" style="1"/>
+    <col min="9" max="9" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16" width="9.140625" style="1"/>
     <col min="17" max="17" width="0" style="1" hidden="1" customWidth="1"/>
     <col min="18" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="45"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="36"/>
       <c r="Q1" s="1">
         <v>15002</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="46"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="48"/>
+      <c r="A2" s="37"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="39"/>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:17" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="25" t="s">
+      <c r="H4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="31" t="s">
+      <c r="J4" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="32"/>
-      <c r="L4" s="32"/>
-      <c r="M4" s="32"/>
-      <c r="N4" s="33"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="32"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="13">
-        <v>100</v>
-      </c>
-      <c r="D5" s="8">
+      <c r="B5" s="10">
         <v>1</v>
       </c>
-      <c r="E5" s="6">
+      <c r="C5" s="1">
+        <v>20</v>
+      </c>
+      <c r="D5" s="6">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4">
         <f>(1+$B$6)^(D5-1)</f>
         <v>1</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="56">
         <f>$B$5/$E$26</f>
-        <v>2.7996107123809133</v>
-      </c>
-      <c r="G5" s="12">
+        <v>2.7996107123809132E-2</v>
+      </c>
+      <c r="G5" s="9">
         <f ca="1">RANDBETWEEN($B$7-($B$7*0.5),$B$7+($B$7*0.1))</f>
-        <v>94</v>
-      </c>
-      <c r="H5" s="5">
+        <v>117</v>
+      </c>
+      <c r="H5" s="3">
         <f ca="1">(G5/$B$7)*F5</f>
-        <v>2.0243338997215834</v>
-      </c>
-      <c r="J5" s="30" t="s">
+        <v>2.519649641142822E-2</v>
+      </c>
+      <c r="J5" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="30"/>
-      <c r="L5" s="30"/>
-      <c r="M5" s="30"/>
-      <c r="N5" s="30"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="40"/>
+      <c r="N5" s="40"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="11">
         <v>0.05</v>
       </c>
-      <c r="D6" s="3">
+      <c r="C6" s="1">
+        <v>19</v>
+      </c>
+      <c r="D6" s="2">
         <v>2</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="5">
         <f>(1+$B$6)^(D6-1)</f>
         <v>1.05</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="57">
         <f>F5*(1+$B$6)</f>
-        <v>2.9395912479999593</v>
-      </c>
-      <c r="G6" s="12">
+        <v>2.9395912479999592E-2</v>
+      </c>
+      <c r="G6" s="9">
         <f t="shared" ref="G6:G25" ca="1" si="0">RANDBETWEEN($B$7-($B$7*0.5),$B$7+($B$7*0.1))</f>
-        <v>132</v>
-      </c>
-      <c r="H6" s="5">
+        <v>106</v>
+      </c>
+      <c r="H6" s="3">
         <f t="shared" ref="H6:H25" ca="1" si="1">(G6/$B$7)*F6</f>
-        <v>2.98481572873842</v>
-      </c>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="26"/>
-      <c r="M6" s="26"/>
-      <c r="N6" s="26"/>
+        <v>2.3968974791384282E-2</v>
+      </c>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="33"/>
+      <c r="M6" s="33"/>
+      <c r="N6" s="33"/>
     </row>
     <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="12">
         <v>130</v>
       </c>
-      <c r="D7" s="3">
+      <c r="C7" s="1">
+        <v>18</v>
+      </c>
+      <c r="D7" s="2">
         <v>3</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="5">
         <f>(1+$B$6)^(D7-1)</f>
         <v>1.1025</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="57">
         <f>F6*(1+$B$6)</f>
-        <v>3.0865708103999574</v>
-      </c>
-      <c r="G7" s="12">
+        <v>3.0865708103999571E-2</v>
+      </c>
+      <c r="G7" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>123</v>
-      </c>
-      <c r="H7" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>2.9203708436861135</v>
-      </c>
-      <c r="J7" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="H7" s="3">
+        <f ca="1">(G7/$B$7)*F7</f>
+        <v>2.113113862504586E-2</v>
+      </c>
+      <c r="J7" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
-      <c r="M7" s="26"/>
-      <c r="N7" s="26"/>
-      <c r="O7" s="18"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="33"/>
+      <c r="O7" s="15"/>
     </row>
     <row r="8" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="16">
         <f>LARGE(D:D,1)</f>
         <v>21</v>
       </c>
-      <c r="D8" s="3">
+      <c r="C8" s="1">
+        <v>17</v>
+      </c>
+      <c r="D8" s="2">
         <v>4</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="5">
         <f>(1+$B$6)^(D8-1)</f>
         <v>1.1576250000000001</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="57">
         <f>F7*(1+$B$6)</f>
-        <v>3.2408993509199555</v>
-      </c>
-      <c r="G8" s="12">
+        <v>3.2408993509199555E-2</v>
+      </c>
+      <c r="G8" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>81</v>
+      </c>
+      <c r="H8" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.0193295955732032E-2</v>
+      </c>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="33"/>
+      <c r="M8" s="33"/>
+      <c r="N8" s="33"/>
+      <c r="O8" s="15"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="17"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="1">
+        <v>16</v>
+      </c>
+      <c r="D9" s="2">
+        <v>5</v>
+      </c>
+      <c r="E9" s="5">
+        <f>(1+$B$6)^(D9-1)</f>
+        <v>1.21550625</v>
+      </c>
+      <c r="F9" s="57">
+        <f>F8*(1+$B$6)</f>
+        <v>3.4029443184659537E-2</v>
+      </c>
+      <c r="G9" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>99</v>
+      </c>
+      <c r="H9" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.5914729809856107E-2</v>
+      </c>
+      <c r="J9" s="33"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="33"/>
+      <c r="N9" s="33"/>
+    </row>
+    <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="33"/>
+      <c r="C10" s="1">
+        <v>15</v>
+      </c>
+      <c r="D10" s="2">
+        <v>6</v>
+      </c>
+      <c r="E10" s="5">
+        <f>(1+$B$6)^(D10-1)</f>
+        <v>1.2762815625000001</v>
+      </c>
+      <c r="F10" s="57">
+        <f t="shared" ref="F6:F25" si="2">F9*(1+$B$6)</f>
+        <v>3.5730915343892514E-2</v>
+      </c>
+      <c r="G10" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>101</v>
+      </c>
+      <c r="H10" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.7760172690254954E-2</v>
+      </c>
+      <c r="J10" s="33"/>
+      <c r="K10" s="33"/>
+      <c r="L10" s="33"/>
+      <c r="M10" s="33"/>
+      <c r="N10" s="33"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="33"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="1">
+        <v>14</v>
+      </c>
+      <c r="D11" s="2">
+        <v>7</v>
+      </c>
+      <c r="E11" s="5">
+        <f>(1+$B$6)^(D11-1)</f>
+        <v>1.340095640625</v>
+      </c>
+      <c r="F11" s="57">
+        <f t="shared" si="2"/>
+        <v>3.7517461111087141E-2</v>
+      </c>
+      <c r="G11" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>131</v>
+      </c>
+      <c r="H11" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>3.7806056965787808E-2</v>
+      </c>
+      <c r="J11" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="K11" s="33"/>
+      <c r="L11" s="33"/>
+      <c r="M11" s="33"/>
+      <c r="N11" s="33"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="33"/>
+      <c r="C12" s="1">
+        <v>13</v>
+      </c>
+      <c r="D12" s="2">
+        <v>8</v>
+      </c>
+      <c r="E12" s="5">
+        <f>(1+$B$6)^(D12-1)</f>
+        <v>1.4071004226562502</v>
+      </c>
+      <c r="F12" s="57">
+        <f t="shared" si="2"/>
+        <v>3.9393334166641501E-2</v>
+      </c>
+      <c r="G12" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>67</v>
+      </c>
+      <c r="H12" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.0302718378192156E-2</v>
+      </c>
+      <c r="J12" s="33"/>
+      <c r="K12" s="33"/>
+      <c r="L12" s="33"/>
+      <c r="M12" s="33"/>
+      <c r="N12" s="33"/>
+    </row>
+    <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="33"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="1">
+        <v>12</v>
+      </c>
+      <c r="D13" s="2">
+        <v>9</v>
+      </c>
+      <c r="E13" s="5">
+        <f>(1+$B$6)^(D13-1)</f>
+        <v>1.4774554437890626</v>
+      </c>
+      <c r="F13" s="57">
+        <f t="shared" si="2"/>
+        <v>4.1363000874973577E-2</v>
+      </c>
+      <c r="G13" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>111</v>
+      </c>
+      <c r="H13" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>3.5317639208631284E-2</v>
+      </c>
+      <c r="J13" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="K13" s="33"/>
+      <c r="L13" s="33"/>
+      <c r="M13" s="33"/>
+      <c r="N13" s="33"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="33"/>
+      <c r="C14" s="1">
+        <v>11</v>
+      </c>
+      <c r="D14" s="2">
+        <v>10</v>
+      </c>
+      <c r="E14" s="5">
+        <f t="shared" ref="E5:E25" si="3">(1+$B$6)^(D14-1)</f>
+        <v>1.5513282159785158</v>
+      </c>
+      <c r="F14" s="57">
+        <f t="shared" si="2"/>
+        <v>4.343115091872226E-2</v>
+      </c>
+      <c r="G14" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>76</v>
+      </c>
+      <c r="H14" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.5390518998637632E-2</v>
+      </c>
+      <c r="J14" s="33"/>
+      <c r="K14" s="33"/>
+      <c r="L14" s="33"/>
+      <c r="M14" s="33"/>
+      <c r="N14" s="33"/>
+    </row>
+    <row r="15" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="33"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="1">
+        <v>10</v>
+      </c>
+      <c r="D15" s="2">
+        <v>11</v>
+      </c>
+      <c r="E15" s="5">
+        <f t="shared" si="3"/>
+        <v>1.6288946267774416</v>
+      </c>
+      <c r="F15" s="57">
+        <f t="shared" si="2"/>
+        <v>4.5602708464658373E-2</v>
+      </c>
+      <c r="G15" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>92</v>
+      </c>
+      <c r="H15" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>3.2272685990373619E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="33"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="1">
+        <v>9</v>
+      </c>
+      <c r="D16" s="2">
+        <v>12</v>
+      </c>
+      <c r="E16" s="5">
+        <f t="shared" si="3"/>
+        <v>1.7103393581163138</v>
+      </c>
+      <c r="F16" s="57">
+        <f t="shared" si="2"/>
+        <v>4.7882843887891297E-2</v>
+      </c>
+      <c r="G16" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>77</v>
+      </c>
+      <c r="H16" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.8361376764366383E-2</v>
+      </c>
+      <c r="J16" s="41" t="str">
+        <f ca="1">"O utilizador fez uma média de "&amp;TEXT(AVERAGE(G5:G25),"0,0")&amp; " minutos/dia desta actividade."</f>
+        <v>O utilizador fez uma média de 108,2 minutos/dia desta actividade.</v>
+      </c>
+      <c r="K16" s="42"/>
+      <c r="L16" s="42"/>
+      <c r="M16" s="42"/>
+      <c r="N16" s="43"/>
+    </row>
+    <row r="17" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="1">
+        <v>8</v>
+      </c>
+      <c r="D17" s="2">
+        <v>13</v>
+      </c>
+      <c r="E17" s="5">
+        <f t="shared" si="3"/>
+        <v>1.7958563260221292</v>
+      </c>
+      <c r="F17" s="57">
+        <f t="shared" si="2"/>
+        <v>5.0276986082285861E-2</v>
+      </c>
+      <c r="G17" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>135</v>
+      </c>
+      <c r="H17" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>5.2210716316219936E-2</v>
+      </c>
+      <c r="J17" s="44"/>
+      <c r="K17" s="45"/>
+      <c r="L17" s="45"/>
+      <c r="M17" s="45"/>
+      <c r="N17" s="46"/>
+    </row>
+    <row r="18" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="33"/>
+      <c r="C18" s="1">
+        <v>7</v>
+      </c>
+      <c r="D18" s="2">
+        <v>14</v>
+      </c>
+      <c r="E18" s="5">
+        <f t="shared" si="3"/>
+        <v>1.885649142323236</v>
+      </c>
+      <c r="F18" s="57">
+        <f t="shared" si="2"/>
+        <v>5.2790835386400156E-2</v>
+      </c>
+      <c r="G18" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>108</v>
+      </c>
+      <c r="H18" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>4.3857001705624746E-2</v>
+      </c>
+      <c r="J18" s="47" t="str">
+        <f ca="1">"A sua forma actual é: "&amp;TEXT(H26,"0,0")&amp;"."</f>
+        <v>A sua forma actual é: 0,9.</v>
+      </c>
+      <c r="K18" s="48"/>
+      <c r="L18" s="48"/>
+      <c r="M18" s="48"/>
+      <c r="N18" s="49"/>
+    </row>
+    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="33"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="1">
+        <v>6</v>
+      </c>
+      <c r="D19" s="2">
+        <v>15</v>
+      </c>
+      <c r="E19" s="5">
+        <f t="shared" si="3"/>
+        <v>1.9799315994393973</v>
+      </c>
+      <c r="F19" s="57">
+        <f t="shared" si="2"/>
+        <v>5.5430377155720169E-2</v>
+      </c>
+      <c r="G19" s="9">
         <f t="shared" ca="1" si="0"/>
         <v>102</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H19" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>2.5428594907218112</v>
-      </c>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
-      <c r="L8" s="26"/>
-      <c r="M8" s="26"/>
-      <c r="N8" s="26"/>
-      <c r="O8" s="18"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
-      <c r="B9" s="21"/>
-      <c r="D9" s="3">
+        <v>4.3491526691411209E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="33"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="1">
         <v>5</v>
       </c>
-      <c r="E9" s="7">
-        <f>(1+$B$6)^(D9-1)</f>
-        <v>1.21550625</v>
-      </c>
-      <c r="F9" s="2">
-        <f>F8*(1+$B$6)</f>
-        <v>3.4029443184659534</v>
-      </c>
-      <c r="G9" s="12">
+      <c r="D20" s="2">
+        <v>16</v>
+      </c>
+      <c r="E20" s="5">
+        <f t="shared" si="3"/>
+        <v>2.0789281794113679</v>
+      </c>
+      <c r="F20" s="57">
+        <f t="shared" si="2"/>
+        <v>5.8201896013506178E-2</v>
+      </c>
+      <c r="G20" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>92</v>
-      </c>
-      <c r="H9" s="5">
+        <v>117</v>
+      </c>
+      <c r="H20" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>2.408237517683598</v>
-      </c>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="26"/>
-    </row>
-    <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="26"/>
-      <c r="D10" s="3">
-        <v>6</v>
-      </c>
-      <c r="E10" s="7">
-        <f>(1+$B$6)^(D10-1)</f>
-        <v>1.2762815625000001</v>
-      </c>
-      <c r="F10" s="2">
-        <f>F9*(1+$B$6)</f>
-        <v>3.5730915343892513</v>
-      </c>
-      <c r="G10" s="12">
+        <v>5.238170641215556E-2</v>
+      </c>
+      <c r="J20" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="K20" s="51"/>
+      <c r="L20" s="51"/>
+      <c r="M20" s="51"/>
+      <c r="N20" s="52"/>
+    </row>
+    <row r="21" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="1">
+        <v>4</v>
+      </c>
+      <c r="D21" s="2">
+        <v>17</v>
+      </c>
+      <c r="E21" s="5">
+        <f t="shared" si="3"/>
+        <v>2.182874588381936</v>
+      </c>
+      <c r="F21" s="57">
+        <f t="shared" si="2"/>
+        <v>6.1111990814181491E-2</v>
+      </c>
+      <c r="G21" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="H10" s="5">
+        <v>136</v>
+      </c>
+      <c r="H21" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>2.7485319495301934</v>
-      </c>
-      <c r="J10" s="26"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="26"/>
-      <c r="N10" s="26"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
-      <c r="B11" s="26"/>
-      <c r="D11" s="3">
-        <v>7</v>
-      </c>
-      <c r="E11" s="7">
-        <f>(1+$B$6)^(D11-1)</f>
-        <v>1.340095640625</v>
-      </c>
-      <c r="F11" s="2">
-        <f>F10*(1+$B$6)</f>
-        <v>3.751746111108714</v>
-      </c>
-      <c r="G11" s="12">
+        <v>6.3932544236374483E-2</v>
+      </c>
+      <c r="J21" s="53"/>
+      <c r="K21" s="54"/>
+      <c r="L21" s="54"/>
+      <c r="M21" s="54"/>
+      <c r="N21" s="55"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C22" s="1">
+        <v>3</v>
+      </c>
+      <c r="D22" s="2">
+        <v>18</v>
+      </c>
+      <c r="E22" s="5">
+        <f t="shared" si="3"/>
+        <v>2.2920183178010332</v>
+      </c>
+      <c r="F22" s="57">
+        <f t="shared" si="2"/>
+        <v>6.4167590354890572E-2</v>
+      </c>
+      <c r="G22" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>125</v>
-      </c>
-      <c r="H11" s="5">
+        <v>120</v>
+      </c>
+      <c r="H22" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>3.6074481837583789</v>
-      </c>
-      <c r="J11" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="K11" s="26"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
-      <c r="N11" s="26"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="26"/>
-      <c r="D12" s="3">
-        <v>8</v>
-      </c>
-      <c r="E12" s="7">
-        <f>(1+$B$6)^(D12-1)</f>
-        <v>1.4071004226562502</v>
-      </c>
-      <c r="F12" s="2">
-        <f>F11*(1+$B$6)</f>
-        <v>3.9393334166641498</v>
-      </c>
-      <c r="G12" s="12">
+        <v>5.9231621866052839E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C23" s="1">
+        <v>2</v>
+      </c>
+      <c r="D23" s="2">
+        <v>19</v>
+      </c>
+      <c r="E23" s="5">
+        <f t="shared" si="3"/>
+        <v>2.4066192336910848</v>
+      </c>
+      <c r="F23" s="57">
+        <f t="shared" si="2"/>
+        <v>6.7375969872635097E-2</v>
+      </c>
+      <c r="G23" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>113</v>
-      </c>
-      <c r="H12" s="5">
+        <v>133</v>
+      </c>
+      <c r="H23" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>3.4241898160234534</v>
-      </c>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="26"/>
-      <c r="N12" s="26"/>
-    </row>
-    <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
-      <c r="B13" s="26"/>
-      <c r="D13" s="3">
-        <v>9</v>
-      </c>
-      <c r="E13" s="7">
-        <f>(1+$B$6)^(D13-1)</f>
-        <v>1.4774554437890626</v>
-      </c>
-      <c r="F13" s="2">
-        <f>F12*(1+$B$6)</f>
-        <v>4.1363000874973572</v>
-      </c>
-      <c r="G13" s="12">
+        <v>6.8930799946618979E-2</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J23" s="1">
+        <f>B8-C23-1</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
+      <c r="D24" s="2">
+        <v>20</v>
+      </c>
+      <c r="E24" s="5">
+        <f t="shared" si="3"/>
+        <v>2.526950195375639</v>
+      </c>
+      <c r="F24" s="57">
+        <f t="shared" si="2"/>
+        <v>7.074476836626685E-2</v>
+      </c>
+      <c r="G24" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="H13" s="5">
+        <v>131</v>
+      </c>
+      <c r="H24" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>3.1817692980748902</v>
-      </c>
-      <c r="J13" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="K13" s="26"/>
-      <c r="L13" s="26"/>
-      <c r="M13" s="26"/>
-      <c r="N13" s="26"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="26"/>
-      <c r="D14" s="3">
-        <v>10</v>
-      </c>
-      <c r="E14" s="7">
-        <f>(1+$B$6)^(D14-1)</f>
-        <v>1.5513282159785158</v>
-      </c>
-      <c r="F14" s="2">
-        <f>F13*(1+$B$6)</f>
-        <v>4.3431150918722254</v>
-      </c>
-      <c r="G14" s="12">
+        <v>7.1288958892161206E-2</v>
+      </c>
+      <c r="J24" s="59">
+        <f>F5*((1+B6)^J23)</f>
+        <v>6.7375969872635055E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="14"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="1">
+        <v>0</v>
+      </c>
+      <c r="D25" s="7">
+        <v>21</v>
+      </c>
+      <c r="E25" s="8">
+        <f t="shared" si="3"/>
+        <v>2.6532977051444209</v>
+      </c>
+      <c r="F25" s="58">
+        <f t="shared" si="2"/>
+        <v>7.428200678458019E-2</v>
+      </c>
+      <c r="G25" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>112</v>
-      </c>
-      <c r="H14" s="5">
+        <v>143</v>
+      </c>
+      <c r="H25" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>3.7417606945360715</v>
-      </c>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="26"/>
-      <c r="M14" s="26"/>
-      <c r="N14" s="26"/>
-    </row>
-    <row r="15" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="26"/>
-      <c r="B15" s="26"/>
-      <c r="D15" s="3">
-        <v>11</v>
-      </c>
-      <c r="E15" s="7">
-        <f>(1+$B$6)^(D15-1)</f>
-        <v>1.6288946267774416</v>
-      </c>
-      <c r="F15" s="2">
-        <f>F14*(1+$B$6)</f>
-        <v>4.560270846465837</v>
-      </c>
-      <c r="G15" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>106</v>
-      </c>
-      <c r="H15" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>3.7183746901952208</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
-      <c r="B16" s="26"/>
-      <c r="D16" s="3">
-        <v>12</v>
-      </c>
-      <c r="E16" s="7">
-        <f>(1+$B$6)^(D16-1)</f>
-        <v>1.7103393581163138</v>
-      </c>
-      <c r="F16" s="2">
-        <f>F15*(1+$B$6)</f>
-        <v>4.7882843887891289</v>
-      </c>
-      <c r="G16" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>132</v>
-      </c>
-      <c r="H16" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.8619503024628079</v>
-      </c>
-      <c r="J16" s="34" t="str">
-        <f ca="1">"O utilizador fez uma média de "&amp;TEXT(AVERAGE(G5:G25),"0,0")&amp; " minutos/dia desta actividade."</f>
-        <v>O utilizador fez uma média de 105,1 minutos/dia desta actividade.</v>
-      </c>
-      <c r="K16" s="35"/>
-      <c r="L16" s="35"/>
-      <c r="M16" s="35"/>
-      <c r="N16" s="36"/>
-    </row>
-    <row r="17" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
-      <c r="D17" s="3">
-        <v>13</v>
-      </c>
-      <c r="E17" s="7">
-        <f>(1+$B$6)^(D17-1)</f>
-        <v>1.7958563260221292</v>
-      </c>
-      <c r="F17" s="2">
-        <f>F16*(1+$B$6)</f>
-        <v>5.0276986082285857</v>
-      </c>
-      <c r="G17" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>127</v>
-      </c>
-      <c r="H17" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.9116747941925416</v>
-      </c>
-      <c r="J17" s="37"/>
-      <c r="K17" s="38"/>
-      <c r="L17" s="38"/>
-      <c r="M17" s="38"/>
-      <c r="N17" s="39"/>
-    </row>
-    <row r="18" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="26"/>
-      <c r="D18" s="3">
-        <v>14</v>
-      </c>
-      <c r="E18" s="7">
-        <f>(1+$B$6)^(D18-1)</f>
-        <v>1.885649142323236</v>
-      </c>
-      <c r="F18" s="2">
-        <f>F17*(1+$B$6)</f>
-        <v>5.2790835386400152</v>
-      </c>
-      <c r="G18" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>118</v>
-      </c>
-      <c r="H18" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.7917835196886296</v>
-      </c>
-      <c r="J18" s="40" t="str">
-        <f ca="1">"A sua forma actual é: "&amp;TEXT(H26,"0,0")&amp;"."</f>
-        <v>A sua forma actual é: 79,1.</v>
-      </c>
-      <c r="K18" s="41"/>
-      <c r="L18" s="41"/>
-      <c r="M18" s="41"/>
-      <c r="N18" s="42"/>
-    </row>
-    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
-      <c r="D19" s="3">
-        <v>15</v>
-      </c>
-      <c r="E19" s="7">
-        <f>(1+$B$6)^(D19-1)</f>
-        <v>1.9799315994393973</v>
-      </c>
-      <c r="F19" s="2">
-        <f>F18*(1+$B$6)</f>
-        <v>5.5430377155720159</v>
-      </c>
-      <c r="G19" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>89</v>
-      </c>
-      <c r="H19" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>3.7948488975839187</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
-      <c r="B20" s="26"/>
-      <c r="D20" s="3">
-        <v>16</v>
-      </c>
-      <c r="E20" s="7">
-        <f>(1+$B$6)^(D20-1)</f>
-        <v>2.0789281794113679</v>
-      </c>
-      <c r="F20" s="2">
-        <f>F19*(1+$B$6)</f>
-        <v>5.8201896013506165</v>
-      </c>
-      <c r="G20" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>67</v>
-      </c>
-      <c r="H20" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>2.9996361791576249</v>
-      </c>
-      <c r="J20" s="49" t="s">
-        <v>20</v>
-      </c>
-      <c r="K20" s="50"/>
-      <c r="L20" s="50"/>
-      <c r="M20" s="50"/>
-      <c r="N20" s="51"/>
-    </row>
-    <row r="21" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D21" s="3">
-        <v>17</v>
-      </c>
-      <c r="E21" s="7">
-        <f>(1+$B$6)^(D21-1)</f>
-        <v>2.182874588381936</v>
-      </c>
-      <c r="F21" s="2">
-        <f>F20*(1+$B$6)</f>
-        <v>6.1111990814181478</v>
-      </c>
-      <c r="G21" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>122</v>
-      </c>
-      <c r="H21" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.735125291792416</v>
-      </c>
-      <c r="J21" s="52"/>
-      <c r="K21" s="53"/>
-      <c r="L21" s="53"/>
-      <c r="M21" s="53"/>
-      <c r="N21" s="54"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D22" s="3">
-        <v>18</v>
-      </c>
-      <c r="E22" s="7">
-        <f>(1+$B$6)^(D22-1)</f>
-        <v>2.2920183178010332</v>
-      </c>
-      <c r="F22" s="2">
-        <f>F21*(1+$B$6)</f>
-        <v>6.4167590354890551</v>
-      </c>
-      <c r="G22" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>80</v>
-      </c>
-      <c r="H22" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>3.9487747910701878</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D23" s="3">
-        <v>19</v>
-      </c>
-      <c r="E23" s="7">
-        <f>(1+$B$6)^(D23-1)</f>
-        <v>2.4066192336910848</v>
-      </c>
-      <c r="F23" s="2">
-        <f>F22*(1+$B$6)</f>
-        <v>6.7375969872635082</v>
-      </c>
-      <c r="G23" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>94</v>
-      </c>
-      <c r="H23" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.871800898482844</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
-      <c r="B24" s="17"/>
-      <c r="D24" s="3">
-        <v>20</v>
-      </c>
-      <c r="E24" s="7">
-        <f>(1+$B$6)^(D24-1)</f>
-        <v>2.526950195375639</v>
-      </c>
-      <c r="F24" s="2">
-        <f>F23*(1+$B$6)</f>
-        <v>7.0744768366266841</v>
-      </c>
-      <c r="G24" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>113</v>
-      </c>
-      <c r="H24" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>6.1493529426062716</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="17"/>
-      <c r="B25" s="17"/>
-      <c r="D25" s="9">
-        <v>21</v>
-      </c>
-      <c r="E25" s="10">
-        <f>(1+$B$6)^(D25-1)</f>
-        <v>2.6532977051444209</v>
-      </c>
-      <c r="F25" s="11">
-        <f>F24*(1+$B$6)</f>
-        <v>7.428200678458019</v>
-      </c>
-      <c r="G25" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>66</v>
-      </c>
-      <c r="H25" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>3.771240344447917</v>
+        <v>8.1710207463038212E-2</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="16"/>
-      <c r="B26" s="16"/>
-      <c r="D26" s="55" t="s">
+      <c r="A26" s="13"/>
+      <c r="B26" s="13"/>
+      <c r="D26" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E26" s="56">
+      <c r="E26" s="27">
         <f>SUM(E5:E25)</f>
         <v>35.719251808032823</v>
       </c>
-      <c r="F26" s="57">
-        <f t="shared" ref="F26:H26" si="2">SUM(F5:F25)</f>
-        <v>100.00000000000006</v>
-      </c>
-      <c r="G26" s="57">
-        <f t="shared" ca="1" si="2"/>
-        <v>2207</v>
-      </c>
-      <c r="H26" s="58">
-        <f t="shared" ca="1" si="2"/>
-        <v>79.138880074154898</v>
+      <c r="F26" s="28">
+        <f t="shared" ref="F26:H26" si="4">SUM(F5:F25)</f>
+        <v>1.0000000000000007</v>
+      </c>
+      <c r="G26" s="28">
+        <f t="shared" ca="1" si="4"/>
+        <v>2272</v>
+      </c>
+      <c r="H26" s="29">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.86065088811934765</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="16"/>
-      <c r="B27" s="16"/>
+      <c r="A27" s="13"/>
+      <c r="B27" s="13"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="16"/>
-      <c r="B28" s="16"/>
+      <c r="A28" s="13"/>
+      <c r="B28" s="13"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="16"/>
-      <c r="B29" s="16"/>
+      <c r="A29" s="13"/>
+      <c r="B29" s="13"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="16"/>
-      <c r="B30" s="16"/>
+      <c r="A30" s="13"/>
+      <c r="B30" s="13"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="16"/>
-      <c r="B31" s="16"/>
+      <c r="A31" s="13"/>
+      <c r="B31" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="J4:N4"/>
-    <mergeCell ref="J11:N12"/>
-    <mergeCell ref="J13:N14"/>
-    <mergeCell ref="A1:I2"/>
-    <mergeCell ref="J5:N6"/>
     <mergeCell ref="A18:B20"/>
     <mergeCell ref="J7:N10"/>
     <mergeCell ref="J16:N17"/>
@@ -1948,6 +2026,11 @@
     <mergeCell ref="A10:B11"/>
     <mergeCell ref="A12:B13"/>
     <mergeCell ref="A14:B17"/>
+    <mergeCell ref="J4:N4"/>
+    <mergeCell ref="J11:N12"/>
+    <mergeCell ref="J13:N14"/>
+    <mergeCell ref="A1:I2"/>
+    <mergeCell ref="J5:N6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1970,8 +2053,8 @@
                   <to>
                     <xdr:col>12</xdr:col>
                     <xdr:colOff>238125</xdr:colOff>
-                    <xdr:row>23</xdr:row>
-                    <xdr:rowOff>190500</xdr:rowOff>
+                    <xdr:row>24</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>

</xml_diff>